<commit_message>
add resources & update README
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a0ca4fbcb46ad72/桌面/IOL/generator_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_AD4DBB64A54DDB1B405E38C3451D34154F90DF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09E5DB9F-2741-4893-BD4A-D5FA6B4D3361}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_AD4DBB64A54DDB1B405E38C3451D34154F90DF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02D71C46-CDB4-4F09-9177-38DE981CE2CD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,10 +428,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.19921875" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>